<commit_message>
- Les données fournies dans les fichiers de l'EERV sont séparées par paroisse avant d'être importées. - Adapté les fichiers d'exemples de la paroisse de Morges. - Adapté les tests unitaires.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@18440 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Morges/Groupes.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Morges/Groupes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
   <si>
     <t>IdxG</t>
   </si>
@@ -530,6 +530,9 @@
   </si>
   <si>
     <t>Petites mains</t>
+  </si>
+  <si>
+    <t>IdxPar</t>
   </si>
 </sst>
 </file>
@@ -1014,8 +1017,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1358,18 +1364,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C171"/>
+  <dimension ref="A1:D171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B169" sqref="B169"/>
+      <selection activeCell="E169" sqref="E169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="41.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1379,8 +1386,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>403110100</v>
       </c>
@@ -1390,8 +1400,11 @@
       <c r="C2">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>403110200</v>
       </c>
@@ -1401,8 +1414,11 @@
       <c r="C3">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>403110300</v>
       </c>
@@ -1412,8 +1428,11 @@
       <c r="C4">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>403110400</v>
       </c>
@@ -1423,8 +1442,11 @@
       <c r="C5">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>403110500</v>
       </c>
@@ -1434,8 +1456,11 @@
       <c r="C6">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>403110600</v>
       </c>
@@ -1445,8 +1470,11 @@
       <c r="C7">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>403110700</v>
       </c>
@@ -1456,8 +1484,11 @@
       <c r="C8">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>403110800</v>
       </c>
@@ -1467,8 +1498,11 @@
       <c r="C9">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>403110900</v>
       </c>
@@ -1478,8 +1512,11 @@
       <c r="C10">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>403111000</v>
       </c>
@@ -1489,8 +1526,11 @@
       <c r="C11">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>403111100</v>
       </c>
@@ -1500,8 +1540,11 @@
       <c r="C12">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>403111200</v>
       </c>
@@ -1511,8 +1554,11 @@
       <c r="C13">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>403111300</v>
       </c>
@@ -1522,8 +1568,11 @@
       <c r="C14">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>403111400</v>
       </c>
@@ -1533,8 +1582,11 @@
       <c r="C15">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>403111500</v>
       </c>
@@ -1544,8 +1596,11 @@
       <c r="C16">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>403111600</v>
       </c>
@@ -1555,8 +1610,11 @@
       <c r="C17">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>403111700</v>
       </c>
@@ -1566,8 +1624,11 @@
       <c r="C18">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>403111800</v>
       </c>
@@ -1577,8 +1638,11 @@
       <c r="C19">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>403111900</v>
       </c>
@@ -1588,8 +1652,11 @@
       <c r="C20">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>403112000</v>
       </c>
@@ -1599,8 +1666,11 @@
       <c r="C21">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>403112100</v>
       </c>
@@ -1610,8 +1680,11 @@
       <c r="C22">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>403112200</v>
       </c>
@@ -1621,8 +1694,11 @@
       <c r="C23">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>403112300</v>
       </c>
@@ -1632,8 +1708,11 @@
       <c r="C24">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>403112400</v>
       </c>
@@ -1643,8 +1722,11 @@
       <c r="C25">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>403112500</v>
       </c>
@@ -1654,8 +1736,11 @@
       <c r="C26">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>403112600</v>
       </c>
@@ -1665,8 +1750,11 @@
       <c r="C27">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>403112700</v>
       </c>
@@ -1676,8 +1764,11 @@
       <c r="C28">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>403112800</v>
       </c>
@@ -1687,8 +1778,11 @@
       <c r="C29">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>403112900</v>
       </c>
@@ -1698,8 +1792,11 @@
       <c r="C30">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>403113000</v>
       </c>
@@ -1709,8 +1806,11 @@
       <c r="C31">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>403113100</v>
       </c>
@@ -1720,8 +1820,11 @@
       <c r="C32">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>403113200</v>
       </c>
@@ -1731,8 +1834,11 @@
       <c r="C33">
         <v>403110000</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>403113301</v>
       </c>
@@ -1742,8 +1848,11 @@
       <c r="C34">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>403113302</v>
       </c>
@@ -1753,8 +1862,11 @@
       <c r="C35">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>403113303</v>
       </c>
@@ -1764,8 +1876,11 @@
       <c r="C36">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>403113304</v>
       </c>
@@ -1775,8 +1890,11 @@
       <c r="C37">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>403113305</v>
       </c>
@@ -1786,8 +1904,11 @@
       <c r="C38">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>403113306</v>
       </c>
@@ -1797,8 +1918,11 @@
       <c r="C39">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>403113308</v>
       </c>
@@ -1808,8 +1932,11 @@
       <c r="C40">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>403113309</v>
       </c>
@@ -1819,8 +1946,11 @@
       <c r="C41">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>403113310</v>
       </c>
@@ -1830,8 +1960,11 @@
       <c r="C42">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>403113311</v>
       </c>
@@ -1841,8 +1974,11 @@
       <c r="C43">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>403113312</v>
       </c>
@@ -1852,8 +1988,11 @@
       <c r="C44">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>403113313</v>
       </c>
@@ -1863,8 +2002,11 @@
       <c r="C45">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>403113314</v>
       </c>
@@ -1874,8 +2016,11 @@
       <c r="C46">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>403113315</v>
       </c>
@@ -1885,8 +2030,11 @@
       <c r="C47">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>403113316</v>
       </c>
@@ -1896,8 +2044,11 @@
       <c r="C48">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>403113317</v>
       </c>
@@ -1907,8 +2058,11 @@
       <c r="C49">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>403113318</v>
       </c>
@@ -1918,8 +2072,11 @@
       <c r="C50">
         <v>403113300</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>403050201</v>
       </c>
@@ -1929,8 +2086,11 @@
       <c r="C51">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>403050202</v>
       </c>
@@ -1940,8 +2100,11 @@
       <c r="C52">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>403050203</v>
       </c>
@@ -1951,8 +2114,11 @@
       <c r="C53">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>403050204</v>
       </c>
@@ -1962,8 +2128,11 @@
       <c r="C54">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>403050205</v>
       </c>
@@ -1973,8 +2142,11 @@
       <c r="C55">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>403050206</v>
       </c>
@@ -1984,8 +2156,11 @@
       <c r="C56">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>403050207</v>
       </c>
@@ -1995,8 +2170,11 @@
       <c r="C57">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>403050208</v>
       </c>
@@ -2006,8 +2184,11 @@
       <c r="C58">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>403050209</v>
       </c>
@@ -2017,8 +2198,11 @@
       <c r="C59">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>403050210</v>
       </c>
@@ -2028,16 +2212,22 @@
       <c r="C60">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>403050211</v>
       </c>
       <c r="C61">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>403050212</v>
       </c>
@@ -2047,8 +2237,11 @@
       <c r="C62">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>403050213</v>
       </c>
@@ -2058,8 +2251,11 @@
       <c r="C63">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>403050214</v>
       </c>
@@ -2069,8 +2265,11 @@
       <c r="C64">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>403050215</v>
       </c>
@@ -2080,8 +2279,11 @@
       <c r="C65">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>403050216</v>
       </c>
@@ -2091,8 +2293,11 @@
       <c r="C66">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>403050217</v>
       </c>
@@ -2102,8 +2307,11 @@
       <c r="C67">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>403050218</v>
       </c>
@@ -2113,8 +2321,11 @@
       <c r="C68">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>403050219</v>
       </c>
@@ -2124,8 +2335,11 @@
       <c r="C69">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>403050220</v>
       </c>
@@ -2135,8 +2349,11 @@
       <c r="C70">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>403050221</v>
       </c>
@@ -2146,8 +2363,11 @@
       <c r="C71">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>403050222</v>
       </c>
@@ -2157,8 +2377,11 @@
       <c r="C72">
         <v>403050200</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>403070200</v>
       </c>
@@ -2168,8 +2391,11 @@
       <c r="C73">
         <v>403070000</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>403070300</v>
       </c>
@@ -2179,8 +2405,11 @@
       <c r="C74">
         <v>403070000</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>403070400</v>
       </c>
@@ -2190,8 +2419,11 @@
       <c r="C75">
         <v>403070000</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>403070500</v>
       </c>
@@ -2201,8 +2433,11 @@
       <c r="C76">
         <v>403070000</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>403070600</v>
       </c>
@@ -2212,8 +2447,11 @@
       <c r="C77">
         <v>403070000</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>403070700</v>
       </c>
@@ -2223,8 +2461,11 @@
       <c r="C78">
         <v>403070000</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>403070800</v>
       </c>
@@ -2234,8 +2475,11 @@
       <c r="C79">
         <v>403070000</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>403070900</v>
       </c>
@@ -2245,8 +2489,11 @@
       <c r="C80">
         <v>403070000</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>403071000</v>
       </c>
@@ -2256,8 +2503,11 @@
       <c r="C81">
         <v>403070000</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>403071100</v>
       </c>
@@ -2267,8 +2517,11 @@
       <c r="C82">
         <v>403070000</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>403071200</v>
       </c>
@@ -2278,8 +2531,11 @@
       <c r="C83">
         <v>403070000</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>403071300</v>
       </c>
@@ -2289,8 +2545,11 @@
       <c r="C84">
         <v>403070000</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>403071400</v>
       </c>
@@ -2300,8 +2559,11 @@
       <c r="C85">
         <v>403070000</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>403090300</v>
       </c>
@@ -2311,8 +2573,11 @@
       <c r="C86">
         <v>403090000</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>403090400</v>
       </c>
@@ -2322,8 +2587,11 @@
       <c r="C87">
         <v>403090000</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>403090500</v>
       </c>
@@ -2333,8 +2601,11 @@
       <c r="C88">
         <v>403090000</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>403090600</v>
       </c>
@@ -2344,8 +2615,11 @@
       <c r="C89">
         <v>403090000</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>403090700</v>
       </c>
@@ -2355,8 +2629,11 @@
       <c r="C90">
         <v>403090000</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>403090800</v>
       </c>
@@ -2366,8 +2643,11 @@
       <c r="C91">
         <v>403090000</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>403090900</v>
       </c>
@@ -2377,8 +2657,11 @@
       <c r="C92">
         <v>403090000</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>403091000</v>
       </c>
@@ -2388,8 +2671,11 @@
       <c r="C93">
         <v>403090000</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>403091100</v>
       </c>
@@ -2399,8 +2685,11 @@
       <c r="C94">
         <v>403090000</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>403091200</v>
       </c>
@@ -2410,8 +2699,11 @@
       <c r="C95">
         <v>403090000</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>403091300</v>
       </c>
@@ -2421,8 +2713,11 @@
       <c r="C96">
         <v>403090000</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>403060102</v>
       </c>
@@ -2432,8 +2727,11 @@
       <c r="C97">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>403060103</v>
       </c>
@@ -2443,8 +2741,11 @@
       <c r="C98">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>403060104</v>
       </c>
@@ -2454,8 +2755,11 @@
       <c r="C99">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>403060105</v>
       </c>
@@ -2465,8 +2769,11 @@
       <c r="C100">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>403060106</v>
       </c>
@@ -2476,8 +2783,11 @@
       <c r="C101">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>403060107</v>
       </c>
@@ -2487,8 +2797,11 @@
       <c r="C102">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>403060108</v>
       </c>
@@ -2498,8 +2811,11 @@
       <c r="C103">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>403060109</v>
       </c>
@@ -2509,8 +2825,11 @@
       <c r="C104">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>403060110</v>
       </c>
@@ -2520,8 +2839,11 @@
       <c r="C105">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>403060111</v>
       </c>
@@ -2531,8 +2853,11 @@
       <c r="C106">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>403060112</v>
       </c>
@@ -2542,8 +2867,11 @@
       <c r="C107">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>403060113</v>
       </c>
@@ -2553,8 +2881,11 @@
       <c r="C108">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>403060114</v>
       </c>
@@ -2564,8 +2895,11 @@
       <c r="C109">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>403060115</v>
       </c>
@@ -2575,8 +2909,11 @@
       <c r="C110">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>403060116</v>
       </c>
@@ -2586,8 +2923,11 @@
       <c r="C111">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>403060117</v>
       </c>
@@ -2597,8 +2937,11 @@
       <c r="C112">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>403060118</v>
       </c>
@@ -2608,8 +2951,11 @@
       <c r="C113">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>403060119</v>
       </c>
@@ -2619,8 +2965,11 @@
       <c r="C114">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>403060120</v>
       </c>
@@ -2630,8 +2979,11 @@
       <c r="C115">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>403060121</v>
       </c>
@@ -2641,8 +2993,11 @@
       <c r="C116">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>403060122</v>
       </c>
@@ -2652,8 +3007,11 @@
       <c r="C117">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>403060123</v>
       </c>
@@ -2663,8 +3021,11 @@
       <c r="C118">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>403060124</v>
       </c>
@@ -2674,8 +3035,11 @@
       <c r="C119">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>403060125</v>
       </c>
@@ -2685,8 +3049,11 @@
       <c r="C120">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>403060126</v>
       </c>
@@ -2696,8 +3063,11 @@
       <c r="C121">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>403060127</v>
       </c>
@@ -2707,8 +3077,11 @@
       <c r="C122">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>403060128</v>
       </c>
@@ -2718,8 +3091,11 @@
       <c r="C123">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>403060129</v>
       </c>
@@ -2729,8 +3105,11 @@
       <c r="C124">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D124" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>403060130</v>
       </c>
@@ -2740,8 +3119,11 @@
       <c r="C125">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>403060131</v>
       </c>
@@ -2751,8 +3133,11 @@
       <c r="C126">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>403060132</v>
       </c>
@@ -2762,8 +3147,11 @@
       <c r="C127">
         <v>403060000</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D127" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>403120100</v>
       </c>
@@ -2773,8 +3161,11 @@
       <c r="C128">
         <v>403120000</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D128" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>403120200</v>
       </c>
@@ -2784,8 +3175,11 @@
       <c r="C129">
         <v>403120000</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D129" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>403120400</v>
       </c>
@@ -2795,8 +3189,11 @@
       <c r="C130">
         <v>403120000</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D130" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>403120500</v>
       </c>
@@ -2806,8 +3203,11 @@
       <c r="C131">
         <v>403120000</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D131" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>403120600</v>
       </c>
@@ -2817,8 +3217,11 @@
       <c r="C132">
         <v>403120000</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D132" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>403120700</v>
       </c>
@@ -2828,8 +3231,11 @@
       <c r="C133">
         <v>403120000</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D133" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>403120800</v>
       </c>
@@ -2839,8 +3245,11 @@
       <c r="C134">
         <v>403120000</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D134" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>403120900</v>
       </c>
@@ -2850,8 +3259,11 @@
       <c r="C135">
         <v>403120000</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D135" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>403121000</v>
       </c>
@@ -2861,8 +3273,11 @@
       <c r="C136">
         <v>403120000</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D136" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>401020100</v>
       </c>
@@ -2872,8 +3287,11 @@
       <c r="C137">
         <v>403030000</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D137" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>403030700</v>
       </c>
@@ -2883,8 +3301,11 @@
       <c r="C138">
         <v>403030000</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D138" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>403030800</v>
       </c>
@@ -2894,8 +3315,11 @@
       <c r="C139">
         <v>403030000</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D139" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>403030900</v>
       </c>
@@ -2905,8 +3329,11 @@
       <c r="C140">
         <v>403030000</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D140" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>403031000</v>
       </c>
@@ -2916,8 +3343,11 @@
       <c r="C141">
         <v>403030000</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>403031100</v>
       </c>
@@ -2927,8 +3357,11 @@
       <c r="C142">
         <v>403030000</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>403031200</v>
       </c>
@@ -2938,8 +3371,11 @@
       <c r="C143">
         <v>403030000</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D143" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>403030500</v>
       </c>
@@ -2949,8 +3385,11 @@
       <c r="C144">
         <v>403030000</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D144" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>403030100</v>
       </c>
@@ -2960,8 +3399,11 @@
       <c r="C145">
         <v>403030000</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D145" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>403030400</v>
       </c>
@@ -2971,8 +3413,11 @@
       <c r="C146">
         <v>403030000</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D146" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>403030200</v>
       </c>
@@ -2982,8 +3427,11 @@
       <c r="C147">
         <v>403030000</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D147" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>403031300</v>
       </c>
@@ -2993,8 +3441,11 @@
       <c r="C148">
         <v>403030000</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D148" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>403031400</v>
       </c>
@@ -3004,8 +3455,11 @@
       <c r="C149">
         <v>403030000</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D149" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>403031500</v>
       </c>
@@ -3015,8 +3469,11 @@
       <c r="C150">
         <v>403030000</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D150" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>403031700</v>
       </c>
@@ -3026,160 +3483,220 @@
       <c r="C151">
         <v>403030000</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D151" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>405010100</v>
       </c>
       <c r="B152" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D152" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>405010200</v>
       </c>
       <c r="B153" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D153" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>405010300</v>
       </c>
       <c r="B154" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D154" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>405010400</v>
       </c>
       <c r="B155" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D155" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>405010800</v>
       </c>
       <c r="B156" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D156" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>405010900</v>
       </c>
       <c r="B157" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D157" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>405011000</v>
       </c>
       <c r="B158" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D158" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>405011100</v>
       </c>
       <c r="B159" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D159" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>405011500</v>
       </c>
       <c r="B160" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D160" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>405012600</v>
       </c>
       <c r="B161" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D161" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>405012700</v>
       </c>
       <c r="B162" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D162" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>405012900</v>
       </c>
       <c r="B163" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D163" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>405013000</v>
       </c>
       <c r="B164" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D164" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>405013400</v>
       </c>
       <c r="B165" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D165" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>405013500</v>
       </c>
       <c r="B166" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D166" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>405013700</v>
       </c>
       <c r="B167" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D167" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>405013900</v>
       </c>
       <c r="B168" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D168" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>405014000</v>
       </c>
       <c r="B169" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D169" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>405014700</v>
       </c>
       <c r="B170" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D170" s="1">
+        <v>9040000000</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>403010201</v>
       </c>
@@ -3188,6 +3705,9 @@
       </c>
       <c r="C171">
         <v>403010200</v>
+      </c>
+      <c r="D171" s="1">
+        <v>9040000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Mis à jour les fichiers d'exemples pour la paroisse de Morges avec les bons numéros d'id de paroisse.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@18470 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Morges/Groupes.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Morges/Groupes.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Groupes2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" refMode="R1C1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -1367,7 +1367,7 @@
   <dimension ref="A1:D171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E169" sqref="E169"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,7 +1401,7 @@
         <v>403110000</v>
       </c>
       <c r="D2" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1415,7 +1415,7 @@
         <v>403110000</v>
       </c>
       <c r="D3" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1429,7 +1429,7 @@
         <v>403110000</v>
       </c>
       <c r="D4" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
         <v>403110000</v>
       </c>
       <c r="D5" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1457,7 +1457,7 @@
         <v>403110000</v>
       </c>
       <c r="D6" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1471,7 +1471,7 @@
         <v>403110000</v>
       </c>
       <c r="D7" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1485,7 +1485,7 @@
         <v>403110000</v>
       </c>
       <c r="D8" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1499,7 +1499,7 @@
         <v>403110000</v>
       </c>
       <c r="D9" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1513,7 +1513,7 @@
         <v>403110000</v>
       </c>
       <c r="D10" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1527,7 +1527,7 @@
         <v>403110000</v>
       </c>
       <c r="D11" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1541,7 +1541,7 @@
         <v>403110000</v>
       </c>
       <c r="D12" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1555,7 +1555,7 @@
         <v>403110000</v>
       </c>
       <c r="D13" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1569,7 +1569,7 @@
         <v>403110000</v>
       </c>
       <c r="D14" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1583,7 +1583,7 @@
         <v>403110000</v>
       </c>
       <c r="D15" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1597,7 +1597,7 @@
         <v>403110000</v>
       </c>
       <c r="D16" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1611,7 +1611,7 @@
         <v>403110000</v>
       </c>
       <c r="D17" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1625,7 +1625,7 @@
         <v>403110000</v>
       </c>
       <c r="D18" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1639,7 +1639,7 @@
         <v>403110000</v>
       </c>
       <c r="D19" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1653,7 +1653,7 @@
         <v>403110000</v>
       </c>
       <c r="D20" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1667,7 +1667,7 @@
         <v>403110000</v>
       </c>
       <c r="D21" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1681,7 +1681,7 @@
         <v>403110000</v>
       </c>
       <c r="D22" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1695,7 +1695,7 @@
         <v>403110000</v>
       </c>
       <c r="D23" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1709,7 +1709,7 @@
         <v>403110000</v>
       </c>
       <c r="D24" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,7 +1723,7 @@
         <v>403110000</v>
       </c>
       <c r="D25" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1737,7 +1737,7 @@
         <v>403110000</v>
       </c>
       <c r="D26" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
         <v>403110000</v>
       </c>
       <c r="D27" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
         <v>403110000</v>
       </c>
       <c r="D28" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1779,7 +1779,7 @@
         <v>403110000</v>
       </c>
       <c r="D29" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1793,7 +1793,7 @@
         <v>403110000</v>
       </c>
       <c r="D30" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1807,7 +1807,7 @@
         <v>403110000</v>
       </c>
       <c r="D31" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1821,7 +1821,7 @@
         <v>403110000</v>
       </c>
       <c r="D32" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1835,7 +1835,7 @@
         <v>403110000</v>
       </c>
       <c r="D33" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1849,7 +1849,7 @@
         <v>403113300</v>
       </c>
       <c r="D34" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1863,7 +1863,7 @@
         <v>403113300</v>
       </c>
       <c r="D35" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1877,7 +1877,7 @@
         <v>403113300</v>
       </c>
       <c r="D36" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1891,7 +1891,7 @@
         <v>403113300</v>
       </c>
       <c r="D37" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1905,7 +1905,7 @@
         <v>403113300</v>
       </c>
       <c r="D38" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1919,7 +1919,7 @@
         <v>403113300</v>
       </c>
       <c r="D39" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1933,7 +1933,7 @@
         <v>403113300</v>
       </c>
       <c r="D40" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
         <v>403113300</v>
       </c>
       <c r="D41" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1961,7 +1961,7 @@
         <v>403113300</v>
       </c>
       <c r="D42" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1975,7 +1975,7 @@
         <v>403113300</v>
       </c>
       <c r="D43" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1989,7 +1989,7 @@
         <v>403113300</v>
       </c>
       <c r="D44" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2003,7 +2003,7 @@
         <v>403113300</v>
       </c>
       <c r="D45" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2017,7 +2017,7 @@
         <v>403113300</v>
       </c>
       <c r="D46" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2031,7 +2031,7 @@
         <v>403113300</v>
       </c>
       <c r="D47" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2045,7 +2045,7 @@
         <v>403113300</v>
       </c>
       <c r="D48" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2059,7 +2059,7 @@
         <v>403113300</v>
       </c>
       <c r="D49" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2073,7 +2073,7 @@
         <v>403113300</v>
       </c>
       <c r="D50" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
         <v>403050200</v>
       </c>
       <c r="D51" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2101,7 +2101,7 @@
         <v>403050200</v>
       </c>
       <c r="D52" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2115,7 +2115,7 @@
         <v>403050200</v>
       </c>
       <c r="D53" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2129,7 +2129,7 @@
         <v>403050200</v>
       </c>
       <c r="D54" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2143,7 +2143,7 @@
         <v>403050200</v>
       </c>
       <c r="D55" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2157,7 +2157,7 @@
         <v>403050200</v>
       </c>
       <c r="D56" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2171,7 +2171,7 @@
         <v>403050200</v>
       </c>
       <c r="D57" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2185,7 +2185,7 @@
         <v>403050200</v>
       </c>
       <c r="D58" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2199,7 +2199,7 @@
         <v>403050200</v>
       </c>
       <c r="D59" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2213,7 +2213,7 @@
         <v>403050200</v>
       </c>
       <c r="D60" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2224,7 +2224,7 @@
         <v>403050200</v>
       </c>
       <c r="D61" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2238,7 +2238,7 @@
         <v>403050200</v>
       </c>
       <c r="D62" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2252,7 +2252,7 @@
         <v>403050200</v>
       </c>
       <c r="D63" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2266,7 +2266,7 @@
         <v>403050200</v>
       </c>
       <c r="D64" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2280,7 +2280,7 @@
         <v>403050200</v>
       </c>
       <c r="D65" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2294,7 +2294,7 @@
         <v>403050200</v>
       </c>
       <c r="D66" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2308,7 +2308,7 @@
         <v>403050200</v>
       </c>
       <c r="D67" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2322,7 +2322,7 @@
         <v>403050200</v>
       </c>
       <c r="D68" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2336,7 +2336,7 @@
         <v>403050200</v>
       </c>
       <c r="D69" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2350,7 +2350,7 @@
         <v>403050200</v>
       </c>
       <c r="D70" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2364,7 +2364,7 @@
         <v>403050200</v>
       </c>
       <c r="D71" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2378,7 +2378,7 @@
         <v>403050200</v>
       </c>
       <c r="D72" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2392,7 +2392,7 @@
         <v>403070000</v>
       </c>
       <c r="D73" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2406,7 +2406,7 @@
         <v>403070000</v>
       </c>
       <c r="D74" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2420,7 +2420,7 @@
         <v>403070000</v>
       </c>
       <c r="D75" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2434,7 +2434,7 @@
         <v>403070000</v>
       </c>
       <c r="D76" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2448,7 +2448,7 @@
         <v>403070000</v>
       </c>
       <c r="D77" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2462,7 +2462,7 @@
         <v>403070000</v>
       </c>
       <c r="D78" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2476,7 +2476,7 @@
         <v>403070000</v>
       </c>
       <c r="D79" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2490,7 +2490,7 @@
         <v>403070000</v>
       </c>
       <c r="D80" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2504,7 +2504,7 @@
         <v>403070000</v>
       </c>
       <c r="D81" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2518,7 +2518,7 @@
         <v>403070000</v>
       </c>
       <c r="D82" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2532,7 +2532,7 @@
         <v>403070000</v>
       </c>
       <c r="D83" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2546,7 +2546,7 @@
         <v>403070000</v>
       </c>
       <c r="D84" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2560,7 +2560,7 @@
         <v>403070000</v>
       </c>
       <c r="D85" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2574,7 +2574,7 @@
         <v>403090000</v>
       </c>
       <c r="D86" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2588,7 +2588,7 @@
         <v>403090000</v>
       </c>
       <c r="D87" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2602,7 +2602,7 @@
         <v>403090000</v>
       </c>
       <c r="D88" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2616,7 +2616,7 @@
         <v>403090000</v>
       </c>
       <c r="D89" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2630,7 +2630,7 @@
         <v>403090000</v>
       </c>
       <c r="D90" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2644,7 +2644,7 @@
         <v>403090000</v>
       </c>
       <c r="D91" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2658,7 +2658,7 @@
         <v>403090000</v>
       </c>
       <c r="D92" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2672,7 +2672,7 @@
         <v>403090000</v>
       </c>
       <c r="D93" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2686,7 +2686,7 @@
         <v>403090000</v>
       </c>
       <c r="D94" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2700,7 +2700,7 @@
         <v>403090000</v>
       </c>
       <c r="D95" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2714,7 +2714,7 @@
         <v>403090000</v>
       </c>
       <c r="D96" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2728,7 +2728,7 @@
         <v>403060000</v>
       </c>
       <c r="D97" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2742,7 +2742,7 @@
         <v>403060000</v>
       </c>
       <c r="D98" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2756,7 +2756,7 @@
         <v>403060000</v>
       </c>
       <c r="D99" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2770,7 +2770,7 @@
         <v>403060000</v>
       </c>
       <c r="D100" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2784,7 +2784,7 @@
         <v>403060000</v>
       </c>
       <c r="D101" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2798,7 +2798,7 @@
         <v>403060000</v>
       </c>
       <c r="D102" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2812,7 +2812,7 @@
         <v>403060000</v>
       </c>
       <c r="D103" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2826,7 +2826,7 @@
         <v>403060000</v>
       </c>
       <c r="D104" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2840,7 +2840,7 @@
         <v>403060000</v>
       </c>
       <c r="D105" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2854,7 +2854,7 @@
         <v>403060000</v>
       </c>
       <c r="D106" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2868,7 +2868,7 @@
         <v>403060000</v>
       </c>
       <c r="D107" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2882,7 +2882,7 @@
         <v>403060000</v>
       </c>
       <c r="D108" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2896,7 +2896,7 @@
         <v>403060000</v>
       </c>
       <c r="D109" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2910,7 +2910,7 @@
         <v>403060000</v>
       </c>
       <c r="D110" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2924,7 +2924,7 @@
         <v>403060000</v>
       </c>
       <c r="D111" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2938,7 +2938,7 @@
         <v>403060000</v>
       </c>
       <c r="D112" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2952,7 +2952,7 @@
         <v>403060000</v>
       </c>
       <c r="D113" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -2966,7 +2966,7 @@
         <v>403060000</v>
       </c>
       <c r="D114" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2980,7 +2980,7 @@
         <v>403060000</v>
       </c>
       <c r="D115" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2994,7 +2994,7 @@
         <v>403060000</v>
       </c>
       <c r="D116" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3008,7 +3008,7 @@
         <v>403060000</v>
       </c>
       <c r="D117" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3022,7 +3022,7 @@
         <v>403060000</v>
       </c>
       <c r="D118" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3036,7 +3036,7 @@
         <v>403060000</v>
       </c>
       <c r="D119" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3050,7 +3050,7 @@
         <v>403060000</v>
       </c>
       <c r="D120" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3064,7 +3064,7 @@
         <v>403060000</v>
       </c>
       <c r="D121" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3078,7 +3078,7 @@
         <v>403060000</v>
       </c>
       <c r="D122" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3092,7 +3092,7 @@
         <v>403060000</v>
       </c>
       <c r="D123" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3106,7 +3106,7 @@
         <v>403060000</v>
       </c>
       <c r="D124" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3120,7 +3120,7 @@
         <v>403060000</v>
       </c>
       <c r="D125" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3134,7 +3134,7 @@
         <v>403060000</v>
       </c>
       <c r="D126" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3148,7 +3148,7 @@
         <v>403060000</v>
       </c>
       <c r="D127" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3162,7 +3162,7 @@
         <v>403120000</v>
       </c>
       <c r="D128" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3176,7 +3176,7 @@
         <v>403120000</v>
       </c>
       <c r="D129" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3190,7 +3190,7 @@
         <v>403120000</v>
       </c>
       <c r="D130" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3204,7 +3204,7 @@
         <v>403120000</v>
       </c>
       <c r="D131" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3218,7 +3218,7 @@
         <v>403120000</v>
       </c>
       <c r="D132" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3232,7 +3232,7 @@
         <v>403120000</v>
       </c>
       <c r="D133" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3246,7 +3246,7 @@
         <v>403120000</v>
       </c>
       <c r="D134" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3260,7 +3260,7 @@
         <v>403120000</v>
       </c>
       <c r="D135" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
         <v>403120000</v>
       </c>
       <c r="D136" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3288,7 +3288,7 @@
         <v>403030000</v>
       </c>
       <c r="D137" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3302,7 +3302,7 @@
         <v>403030000</v>
       </c>
       <c r="D138" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3316,7 +3316,7 @@
         <v>403030000</v>
       </c>
       <c r="D139" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3330,7 +3330,7 @@
         <v>403030000</v>
       </c>
       <c r="D140" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3344,7 +3344,7 @@
         <v>403030000</v>
       </c>
       <c r="D141" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3358,7 +3358,7 @@
         <v>403030000</v>
       </c>
       <c r="D142" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3372,7 +3372,7 @@
         <v>403030000</v>
       </c>
       <c r="D143" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -3386,7 +3386,7 @@
         <v>403030000</v>
       </c>
       <c r="D144" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3400,7 +3400,7 @@
         <v>403030000</v>
       </c>
       <c r="D145" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3414,7 +3414,7 @@
         <v>403030000</v>
       </c>
       <c r="D146" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -3428,7 +3428,7 @@
         <v>403030000</v>
       </c>
       <c r="D147" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -3442,7 +3442,7 @@
         <v>403030000</v>
       </c>
       <c r="D148" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -3456,7 +3456,7 @@
         <v>403030000</v>
       </c>
       <c r="D149" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -3470,7 +3470,7 @@
         <v>403030000</v>
       </c>
       <c r="D150" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -3484,7 +3484,7 @@
         <v>403030000</v>
       </c>
       <c r="D151" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -3495,7 +3495,7 @@
         <v>152</v>
       </c>
       <c r="D152" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -3506,7 +3506,7 @@
         <v>153</v>
       </c>
       <c r="D153" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -3517,7 +3517,7 @@
         <v>154</v>
       </c>
       <c r="D154" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -3528,7 +3528,7 @@
         <v>155</v>
       </c>
       <c r="D155" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -3539,7 +3539,7 @@
         <v>156</v>
       </c>
       <c r="D156" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -3550,7 +3550,7 @@
         <v>157</v>
       </c>
       <c r="D157" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -3561,7 +3561,7 @@
         <v>158</v>
       </c>
       <c r="D158" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -3572,7 +3572,7 @@
         <v>159</v>
       </c>
       <c r="D159" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -3583,7 +3583,7 @@
         <v>160</v>
       </c>
       <c r="D160" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -3594,7 +3594,7 @@
         <v>161</v>
       </c>
       <c r="D161" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -3605,7 +3605,7 @@
         <v>162</v>
       </c>
       <c r="D162" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -3616,7 +3616,7 @@
         <v>163</v>
       </c>
       <c r="D163" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -3627,7 +3627,7 @@
         <v>164</v>
       </c>
       <c r="D164" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -3638,7 +3638,7 @@
         <v>165</v>
       </c>
       <c r="D165" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -3649,7 +3649,7 @@
         <v>166</v>
       </c>
       <c r="D166" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -3660,7 +3660,7 @@
         <v>167</v>
       </c>
       <c r="D167" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -3671,7 +3671,7 @@
         <v>168</v>
       </c>
       <c r="D168" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -3682,7 +3682,7 @@
         <v>169</v>
       </c>
       <c r="D169" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -3693,7 +3693,7 @@
         <v>170</v>
       </c>
       <c r="D170" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -3707,7 +3707,7 @@
         <v>403010200</v>
       </c>
       <c r="D171" s="1">
-        <v>9040000000</v>
+        <v>2010000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Ajout d'un groupe dans les données d'exemples de la paroisse de Morges pour raison de consistance.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@18517 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Morges/Groupes.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Morges/Groupes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
   <si>
     <t>IdxG</t>
   </si>
@@ -533,6 +533,9 @@
   </si>
   <si>
     <t>IdxPar</t>
+  </si>
+  <si>
+    <t>Groupes libres</t>
   </si>
 </sst>
 </file>
@@ -1364,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D171"/>
+  <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2719,10 +2722,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>403060102</v>
+        <v>403060100</v>
       </c>
       <c r="B97" t="s">
-        <v>97</v>
+        <v>173</v>
       </c>
       <c r="C97">
         <v>403060000</v>
@@ -2733,13 +2736,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>403060103</v>
+        <v>403060102</v>
       </c>
       <c r="B98" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C98">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D98" s="1">
         <v>2010000000</v>
@@ -2747,13 +2750,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>403060104</v>
+        <v>403060103</v>
       </c>
       <c r="B99" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C99">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D99" s="1">
         <v>2010000000</v>
@@ -2761,13 +2764,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>403060105</v>
+        <v>403060104</v>
       </c>
       <c r="B100" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C100">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D100" s="1">
         <v>2010000000</v>
@@ -2775,13 +2778,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>403060106</v>
+        <v>403060105</v>
       </c>
       <c r="B101" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C101">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D101" s="1">
         <v>2010000000</v>
@@ -2789,13 +2792,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>403060107</v>
+        <v>403060106</v>
       </c>
       <c r="B102" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C102">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D102" s="1">
         <v>2010000000</v>
@@ -2803,13 +2806,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>403060108</v>
+        <v>403060107</v>
       </c>
       <c r="B103" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C103">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D103" s="1">
         <v>2010000000</v>
@@ -2817,13 +2820,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>403060109</v>
+        <v>403060108</v>
       </c>
       <c r="B104" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C104">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D104" s="1">
         <v>2010000000</v>
@@ -2831,13 +2834,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>403060110</v>
+        <v>403060109</v>
       </c>
       <c r="B105" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C105">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D105" s="1">
         <v>2010000000</v>
@@ -2845,13 +2848,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>403060111</v>
+        <v>403060110</v>
       </c>
       <c r="B106" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C106">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D106" s="1">
         <v>2010000000</v>
@@ -2859,13 +2862,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>403060112</v>
+        <v>403060111</v>
       </c>
       <c r="B107" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C107">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D107" s="1">
         <v>2010000000</v>
@@ -2873,13 +2876,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>403060113</v>
+        <v>403060112</v>
       </c>
       <c r="B108" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C108">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D108" s="1">
         <v>2010000000</v>
@@ -2887,13 +2890,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>403060114</v>
+        <v>403060113</v>
       </c>
       <c r="B109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C109">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D109" s="1">
         <v>2010000000</v>
@@ -2901,13 +2904,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>403060115</v>
+        <v>403060114</v>
       </c>
       <c r="B110" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C110">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D110" s="1">
         <v>2010000000</v>
@@ -2915,13 +2918,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>403060116</v>
+        <v>403060115</v>
       </c>
       <c r="B111" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C111">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D111" s="1">
         <v>2010000000</v>
@@ -2929,13 +2932,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>403060117</v>
+        <v>403060116</v>
       </c>
       <c r="B112" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C112">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D112" s="1">
         <v>2010000000</v>
@@ -2943,13 +2946,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>403060118</v>
+        <v>403060117</v>
       </c>
       <c r="B113" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C113">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D113" s="1">
         <v>2010000000</v>
@@ -2957,13 +2960,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>403060119</v>
+        <v>403060118</v>
       </c>
       <c r="B114" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C114">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D114" s="1">
         <v>2010000000</v>
@@ -2971,13 +2974,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>403060120</v>
+        <v>403060119</v>
       </c>
       <c r="B115" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C115">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D115" s="1">
         <v>2010000000</v>
@@ -2985,13 +2988,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>403060121</v>
+        <v>403060120</v>
       </c>
       <c r="B116" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C116">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D116" s="1">
         <v>2010000000</v>
@@ -2999,13 +3002,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>403060122</v>
+        <v>403060121</v>
       </c>
       <c r="B117" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C117">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D117" s="1">
         <v>2010000000</v>
@@ -3013,13 +3016,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>403060123</v>
+        <v>403060122</v>
       </c>
       <c r="B118" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C118">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D118" s="1">
         <v>2010000000</v>
@@ -3027,13 +3030,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>403060124</v>
+        <v>403060123</v>
       </c>
       <c r="B119" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C119">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D119" s="1">
         <v>2010000000</v>
@@ -3041,13 +3044,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>403060125</v>
+        <v>403060124</v>
       </c>
       <c r="B120" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C120">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D120" s="1">
         <v>2010000000</v>
@@ -3055,13 +3058,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>403060126</v>
+        <v>403060125</v>
       </c>
       <c r="B121" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C121">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D121" s="1">
         <v>2010000000</v>
@@ -3069,13 +3072,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>403060127</v>
+        <v>403060126</v>
       </c>
       <c r="B122" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C122">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D122" s="1">
         <v>2010000000</v>
@@ -3083,13 +3086,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>403060128</v>
+        <v>403060127</v>
       </c>
       <c r="B123" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C123">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D123" s="1">
         <v>2010000000</v>
@@ -3097,13 +3100,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>403060129</v>
+        <v>403060128</v>
       </c>
       <c r="B124" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C124">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D124" s="1">
         <v>2010000000</v>
@@ -3111,13 +3114,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>403060130</v>
+        <v>403060129</v>
       </c>
       <c r="B125" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C125">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D125" s="1">
         <v>2010000000</v>
@@ -3125,13 +3128,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>403060131</v>
+        <v>403060130</v>
       </c>
       <c r="B126" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C126">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D126" s="1">
         <v>2010000000</v>
@@ -3139,13 +3142,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>403060132</v>
+        <v>403060131</v>
       </c>
       <c r="B127" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C127">
-        <v>403060000</v>
+        <v>403060100</v>
       </c>
       <c r="D127" s="1">
         <v>2010000000</v>
@@ -3153,13 +3156,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>403120100</v>
+        <v>403060132</v>
       </c>
       <c r="B128" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C128">
-        <v>403120000</v>
+        <v>403060100</v>
       </c>
       <c r="D128" s="1">
         <v>2010000000</v>
@@ -3167,10 +3170,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>403120200</v>
+        <v>403120100</v>
       </c>
       <c r="B129" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C129">
         <v>403120000</v>
@@ -3181,10 +3184,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>403120400</v>
+        <v>403120200</v>
       </c>
       <c r="B130" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C130">
         <v>403120000</v>
@@ -3195,10 +3198,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>403120500</v>
+        <v>403120400</v>
       </c>
       <c r="B131" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C131">
         <v>403120000</v>
@@ -3209,10 +3212,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>403120600</v>
+        <v>403120500</v>
       </c>
       <c r="B132" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C132">
         <v>403120000</v>
@@ -3223,10 +3226,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>403120700</v>
+        <v>403120600</v>
       </c>
       <c r="B133" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C133">
         <v>403120000</v>
@@ -3237,10 +3240,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>403120800</v>
+        <v>403120700</v>
       </c>
       <c r="B134" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C134">
         <v>403120000</v>
@@ -3251,10 +3254,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>403120900</v>
+        <v>403120800</v>
       </c>
       <c r="B135" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C135">
         <v>403120000</v>
@@ -3265,10 +3268,10 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>403121000</v>
+        <v>403120900</v>
       </c>
       <c r="B136" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C136">
         <v>403120000</v>
@@ -3279,13 +3282,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>401020100</v>
+        <v>403121000</v>
       </c>
       <c r="B137" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C137">
-        <v>403030000</v>
+        <v>403120000</v>
       </c>
       <c r="D137" s="1">
         <v>2010000000</v>
@@ -3293,10 +3296,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>403030700</v>
+        <v>401020100</v>
       </c>
       <c r="B138" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C138">
         <v>403030000</v>
@@ -3307,10 +3310,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>403030800</v>
+        <v>403030700</v>
       </c>
       <c r="B139" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C139">
         <v>403030000</v>
@@ -3321,10 +3324,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>403030900</v>
+        <v>403030800</v>
       </c>
       <c r="B140" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C140">
         <v>403030000</v>
@@ -3335,10 +3338,10 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>403031000</v>
+        <v>403030900</v>
       </c>
       <c r="B141" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C141">
         <v>403030000</v>
@@ -3349,10 +3352,10 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>403031100</v>
+        <v>403031000</v>
       </c>
       <c r="B142" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C142">
         <v>403030000</v>
@@ -3363,10 +3366,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>403031200</v>
+        <v>403031100</v>
       </c>
       <c r="B143" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C143">
         <v>403030000</v>
@@ -3377,10 +3380,10 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>403030500</v>
+        <v>403031200</v>
       </c>
       <c r="B144" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C144">
         <v>403030000</v>
@@ -3391,10 +3394,10 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>403030100</v>
+        <v>403030500</v>
       </c>
       <c r="B145" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C145">
         <v>403030000</v>
@@ -3405,10 +3408,10 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>403030400</v>
+        <v>403030100</v>
       </c>
       <c r="B146" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C146">
         <v>403030000</v>
@@ -3419,10 +3422,10 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>403030200</v>
+        <v>403030400</v>
       </c>
       <c r="B147" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C147">
         <v>403030000</v>
@@ -3433,10 +3436,10 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>403031300</v>
+        <v>403030200</v>
       </c>
       <c r="B148" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C148">
         <v>403030000</v>
@@ -3447,10 +3450,10 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>403031400</v>
+        <v>403031300</v>
       </c>
       <c r="B149" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C149">
         <v>403030000</v>
@@ -3461,10 +3464,10 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>403031500</v>
+        <v>403031400</v>
       </c>
       <c r="B150" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C150">
         <v>403030000</v>
@@ -3475,10 +3478,10 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>403031700</v>
+        <v>403031500</v>
       </c>
       <c r="B151" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C151">
         <v>403030000</v>
@@ -3489,10 +3492,13 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>405010100</v>
+        <v>403031700</v>
       </c>
       <c r="B152" t="s">
-        <v>152</v>
+        <v>151</v>
+      </c>
+      <c r="C152">
+        <v>403030000</v>
       </c>
       <c r="D152" s="1">
         <v>2010000000</v>
@@ -3500,10 +3506,10 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>405010200</v>
+        <v>405010100</v>
       </c>
       <c r="B153" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D153" s="1">
         <v>2010000000</v>
@@ -3511,10 +3517,10 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>405010300</v>
+        <v>405010200</v>
       </c>
       <c r="B154" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D154" s="1">
         <v>2010000000</v>
@@ -3522,10 +3528,10 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>405010400</v>
+        <v>405010300</v>
       </c>
       <c r="B155" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D155" s="1">
         <v>2010000000</v>
@@ -3533,10 +3539,10 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>405010800</v>
+        <v>405010400</v>
       </c>
       <c r="B156" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D156" s="1">
         <v>2010000000</v>
@@ -3544,10 +3550,10 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>405010900</v>
+        <v>405010800</v>
       </c>
       <c r="B157" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D157" s="1">
         <v>2010000000</v>
@@ -3555,10 +3561,10 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>405011000</v>
+        <v>405010900</v>
       </c>
       <c r="B158" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D158" s="1">
         <v>2010000000</v>
@@ -3566,10 +3572,10 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>405011100</v>
+        <v>405011000</v>
       </c>
       <c r="B159" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D159" s="1">
         <v>2010000000</v>
@@ -3577,10 +3583,10 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>405011500</v>
+        <v>405011100</v>
       </c>
       <c r="B160" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D160" s="1">
         <v>2010000000</v>
@@ -3588,10 +3594,10 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>405012600</v>
+        <v>405011500</v>
       </c>
       <c r="B161" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D161" s="1">
         <v>2010000000</v>
@@ -3599,10 +3605,10 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>405012700</v>
+        <v>405012600</v>
       </c>
       <c r="B162" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D162" s="1">
         <v>2010000000</v>
@@ -3610,10 +3616,10 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>405012900</v>
+        <v>405012700</v>
       </c>
       <c r="B163" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D163" s="1">
         <v>2010000000</v>
@@ -3621,10 +3627,10 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>405013000</v>
+        <v>405012900</v>
       </c>
       <c r="B164" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D164" s="1">
         <v>2010000000</v>
@@ -3632,10 +3638,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>405013400</v>
+        <v>405013000</v>
       </c>
       <c r="B165" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D165" s="1">
         <v>2010000000</v>
@@ -3643,10 +3649,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>405013500</v>
+        <v>405013400</v>
       </c>
       <c r="B166" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D166" s="1">
         <v>2010000000</v>
@@ -3654,10 +3660,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>405013700</v>
+        <v>405013500</v>
       </c>
       <c r="B167" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D167" s="1">
         <v>2010000000</v>
@@ -3665,10 +3671,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>405013900</v>
+        <v>405013700</v>
       </c>
       <c r="B168" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D168" s="1">
         <v>2010000000</v>
@@ -3676,10 +3682,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>405014000</v>
+        <v>405013900</v>
       </c>
       <c r="B169" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D169" s="1">
         <v>2010000000</v>
@@ -3687,10 +3693,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>405014700</v>
+        <v>405014000</v>
       </c>
       <c r="B170" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D170" s="1">
         <v>2010000000</v>
@@ -3698,15 +3704,26 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171">
+        <v>405014700</v>
+      </c>
+      <c r="B171" t="s">
+        <v>170</v>
+      </c>
+      <c r="D171" s="1">
+        <v>2010000000</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172">
         <v>403010201</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B172" t="s">
         <v>171</v>
       </c>
-      <c r="C171">
+      <c r="C172">
         <v>403010200</v>
       </c>
-      <c r="D171" s="1">
+      <c r="D172" s="1">
         <v>2010000000</v>
       </c>
     </row>

</xml_diff>